<commit_message>
feat: merchant id for each table, delete: row password for import user from excel
</commit_message>
<xml_diff>
--- a/public/template/template_Peserta.xlsx
+++ b/public/template/template_Peserta.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nama</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Asal Institusi</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Budi Santoso</t>
   </si>
   <si>
@@ -35,9 +32,6 @@
   </si>
   <si>
     <t>Universitas Teknologi Bandung</t>
-  </si>
-  <si>
-    <t>password123</t>
   </si>
   <si>
     <t>Ani Wijaya</t>
@@ -49,9 +43,6 @@
     <t>Institut Seni Rupa Bandung</t>
   </si>
   <si>
-    <t>rahasia456</t>
-  </si>
-  <si>
     <t>Chandra Liem</t>
   </si>
   <si>
@@ -60,15 +51,12 @@
   <si>
     <t>SMA Harapan Bangsa</t>
   </si>
-  <si>
-    <t>pass&amp;word789</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -80,6 +68,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="24.0"/>
       <color theme="1"/>
@@ -98,7 +87,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
@@ -114,20 +103,42 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -357,70 +368,62 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <f>6281234567890</f>
         <v>6281234567890</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5">
+        <v>6.287712345678E12</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6.287712345678E12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5">
         <v>6.285698765432E12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1"/>
@@ -1419,6 +1422,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>